<commit_message>
Lume: some bug fixes.
</commit_message>
<xml_diff>
--- a/Lume/Lume.xlsx
+++ b/Lume/Lume.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="345" windowWidth="17955" windowHeight="8220" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="345" windowWidth="17955" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="275">
   <si>
     <t>Crystal freq</t>
   </si>
@@ -803,6 +803,63 @@
   </si>
   <si>
     <t>XTAL1</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>12 и 11</t>
+  </si>
+  <si>
+    <t>1 и 12</t>
+  </si>
+  <si>
+    <t>2 и 1</t>
+  </si>
+  <si>
+    <t>3 и 2</t>
+  </si>
+  <si>
+    <t>10 и 9</t>
+  </si>
+  <si>
+    <t>11 и 10</t>
+  </si>
+  <si>
+    <t>Hyperminute</t>
+  </si>
+  <si>
+    <t>12 и 11.5</t>
+  </si>
+  <si>
+    <t>0.5 и 0</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>1 и 0.5</t>
+  </si>
+  <si>
+    <t>F CPU</t>
+  </si>
+  <si>
+    <t>MHz</t>
+  </si>
+  <si>
+    <t>Timer input freq</t>
+  </si>
+  <si>
+    <t>Timer ovf freq</t>
+  </si>
+  <si>
+    <t>Divisor</t>
+  </si>
+  <si>
+    <t>ICR</t>
+  </si>
+  <si>
+    <t>OVF freq</t>
   </si>
 </sst>
 </file>
@@ -1291,18 +1348,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1313,7 +1371,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1321,7 +1379,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1333,7 +1391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1342,12 +1400,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1358,7 +1416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1366,7 +1424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1378,7 +1436,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -1390,7 +1448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1402,7 +1460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
@@ -1410,7 +1468,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1421,12 +1479,8 @@
       <c r="C15" t="s">
         <v>14</v>
       </c>
-      <c r="G15">
-        <f>0.197*360</f>
-        <v>70.92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
@@ -1436,6 +1490,274 @@
       </c>
       <c r="C16" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>256</v>
+      </c>
+      <c r="G20" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>257</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>258</v>
+      </c>
+      <c r="G22">
+        <f>G21+1</f>
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>265</v>
+      </c>
+      <c r="I22" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>259</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G44" si="0">G22+1</f>
+        <v>2</v>
+      </c>
+      <c r="H23" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>260</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>9</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>261</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>268</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>269</v>
+      </c>
+      <c r="D32">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>262</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>271</v>
+      </c>
+      <c r="B33">
+        <f>B32*1000000/256</f>
+        <v>3906.25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>272</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>270</v>
+      </c>
+      <c r="B39">
+        <f>B32*1000000/B38</f>
+        <v>1000000</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39">
+        <f>G38+1</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>273</v>
+      </c>
+      <c r="B40">
+        <v>255</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>274</v>
+      </c>
+      <c r="B41">
+        <f>B39/B40</f>
+        <v>3921.5686274509803</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <f>G41+1</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <f t="shared" si="0"/>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1447,7 +1769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Lume: brightness adjustment implemented.
</commit_message>
<xml_diff>
--- a/Lume/Lume.xlsx
+++ b/Lume/Lume.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="259">
   <si>
     <t>Crystal freq</t>
   </si>
@@ -49,42 +49,9 @@
     <t>OVFs per second</t>
   </si>
   <si>
-    <t>Register-based schema</t>
-  </si>
-  <si>
-    <t>LED number</t>
-  </si>
-  <si>
     <t>Hz</t>
   </si>
   <si>
-    <t>SPI freq</t>
-  </si>
-  <si>
-    <t>F cpu</t>
-  </si>
-  <si>
-    <t>bit duration</t>
-  </si>
-  <si>
-    <t>us</t>
-  </si>
-  <si>
-    <t>Packet duration</t>
-  </si>
-  <si>
-    <t>PWM resolution</t>
-  </si>
-  <si>
-    <t>PWM period</t>
-  </si>
-  <si>
-    <t>ms</t>
-  </si>
-  <si>
-    <t>PWM freq</t>
-  </si>
-  <si>
     <t>Цена</t>
   </si>
   <si>
@@ -805,54 +772,9 @@
     <t>XTAL1</t>
   </si>
   <si>
-    <t>Hour</t>
-  </si>
-  <si>
-    <t>12 и 11</t>
-  </si>
-  <si>
-    <t>1 и 12</t>
-  </si>
-  <si>
-    <t>2 и 1</t>
-  </si>
-  <si>
-    <t>3 и 2</t>
-  </si>
-  <si>
-    <t>10 и 9</t>
-  </si>
-  <si>
-    <t>11 и 10</t>
-  </si>
-  <si>
-    <t>Hyperminute</t>
-  </si>
-  <si>
-    <t>12 и 11.5</t>
-  </si>
-  <si>
-    <t>0.5 и 0</t>
-  </si>
-  <si>
-    <t>!</t>
-  </si>
-  <si>
-    <t>1 и 0.5</t>
-  </si>
-  <si>
-    <t>F CPU</t>
-  </si>
-  <si>
-    <t>MHz</t>
-  </si>
-  <si>
     <t>Timer input freq</t>
   </si>
   <si>
-    <t>Timer ovf freq</t>
-  </si>
-  <si>
     <t>Divisor</t>
   </si>
   <si>
@@ -860,12 +782,45 @@
   </si>
   <si>
     <t>OVF freq</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>mV</t>
+  </si>
+  <si>
+    <t>ADC MAX</t>
+  </si>
+  <si>
+    <t>ADC step</t>
+  </si>
+  <si>
+    <t>mv/step</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>ADC value</t>
+  </si>
+  <si>
+    <t>steps</t>
+  </si>
+  <si>
+    <t>Steps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1024,13 +979,11 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1038,6 +991,8 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
@@ -1348,10 +1303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,403 +1316,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="1">
         <v>32768</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <f>B1/B2</f>
         <v>256</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <f>B3/256</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>245</v>
+      </c>
+      <c r="B9" t="e">
+        <f>#REF!*1000000/B8</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1000000</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1">
-        <v>36</v>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>247</v>
+      </c>
+      <c r="B10">
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3">
-        <f>B9/2</f>
-        <v>500000</v>
+      <c r="A11" t="s">
+        <v>248</v>
+      </c>
+      <c r="B11" t="e">
+        <f>B9/B10</f>
+        <v>#REF!</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="3">
-        <f>1000000/B11</f>
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3">
-        <f>B10*B12</f>
-        <v>72</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3">
-        <f>B13*B14/1000</f>
-        <v>7.2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4">
-        <f>1000/B15</f>
-        <v>138.88888888888889</v>
+      <c r="A16" t="s">
+        <v>250</v>
+      </c>
+      <c r="B16">
+        <v>5000</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>252</v>
+      </c>
+      <c r="B17">
+        <v>255</v>
+      </c>
+      <c r="C17" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18" s="9">
+        <f>B16/B17</f>
+        <v>19.607843137254903</v>
+      </c>
+      <c r="C18" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19">
+        <v>3900</v>
+      </c>
+      <c r="C19" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="G20" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="B20" s="3">
+        <f>B19/B18</f>
+        <v>198.89999999999998</v>
+      </c>
+      <c r="C20" t="s">
         <v>257</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>258</v>
       </c>
-      <c r="G22">
-        <f>G21+1</f>
-        <v>1</v>
-      </c>
-      <c r="H22" t="s">
-        <v>265</v>
-      </c>
-      <c r="I22" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D23">
-        <v>2</v>
-      </c>
-      <c r="E23" t="s">
-        <v>259</v>
-      </c>
-      <c r="G23">
-        <f t="shared" ref="G23:G44" si="0">G22+1</f>
-        <v>2</v>
-      </c>
-      <c r="H23" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D24">
-        <v>3</v>
-      </c>
-      <c r="E24" t="s">
-        <v>260</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D25">
-        <v>4</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D26">
-        <v>5</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D27">
-        <v>6</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D28">
-        <v>7</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D29">
-        <v>8</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D30">
-        <v>9</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D31">
-        <v>10</v>
-      </c>
-      <c r="E31" t="s">
-        <v>261</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>268</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>269</v>
-      </c>
-      <c r="D32">
-        <v>11</v>
-      </c>
-      <c r="E32" t="s">
-        <v>262</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>271</v>
-      </c>
-      <c r="B33">
-        <f>B32*1000000/256</f>
-        <v>3906.25</v>
-      </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="G33">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G34">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G35">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G36">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G37">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>272</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>270</v>
-      </c>
-      <c r="B39">
-        <f>B32*1000000/B38</f>
-        <v>1000000</v>
-      </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="G39">
-        <f>G38+1</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>273</v>
-      </c>
-      <c r="B40">
+      <c r="B22">
+        <v>200</v>
+      </c>
+      <c r="C22" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="G40">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>274</v>
-      </c>
-      <c r="B41">
-        <f>B39/B40</f>
-        <v>3921.5686274509803</v>
-      </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="G41">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G42">
-        <f>G41+1</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G43">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G44">
-        <f t="shared" si="0"/>
-        <v>23</v>
+      <c r="B23" s="10">
+        <f>B22*B18</f>
+        <v>3921.5686274509808</v>
+      </c>
+      <c r="C23" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -1779,31 +1499,31 @@
     <col min="5" max="5" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="8" t="s">
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>90</v>
@@ -1818,7 +1538,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1830,7 +1550,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>6</v>
@@ -1840,14 +1560,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>32</v>
+    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>0.2</v>
@@ -1862,7 +1582,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>0.2</v>
@@ -1875,14 +1595,14 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>35</v>
+    <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>0.1</v>
@@ -1897,7 +1617,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <v>0.2</v>
@@ -1910,14 +1630,14 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>38</v>
+    <row r="12" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -1932,7 +1652,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>200</v>
@@ -1947,7 +1667,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1962,7 +1682,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -1977,9 +1697,9 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="9">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7">
         <v>20</v>
       </c>
       <c r="C17">
@@ -1992,7 +1712,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>25</v>
@@ -2007,7 +1727,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2015,7 +1735,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2023,7 +1743,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -2038,7 +1758,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D24">
         <f>SUM(D3:D22)</f>
@@ -2068,1453 +1788,1453 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B52" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B56" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B58" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B59" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B61" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B62" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B67" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B68" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B69" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B70" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B71" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B73" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B74" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B75" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B76" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B77" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B78" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B79" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B80" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B81" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B82" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B83" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B84" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B85" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B86" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B87" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B88" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B89" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B90" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="B91" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B92" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B93" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B94" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B95" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B96" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B97" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B98" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="B99" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B100" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B101" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="B102" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B103" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B104" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B105" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B106" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B107" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B108" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="B109" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B110" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B111" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="B112" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B113" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B114" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B115" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B116" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B117" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B118" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B119" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B120" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B121" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B122" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B123" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B124" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B125" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B126" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B127" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B128" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B129" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B130" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B131" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B132" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B133" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B134" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B135" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B136" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B137" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B138" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B139" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B140" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="B141" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B142" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B143" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B144" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B145" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="B146" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="B147" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="B148" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B149" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B150" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B151" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="B152" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B153" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B154" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="B155" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B156" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B157" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="B158" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B159" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="B160" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B161" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="B162" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="B163" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B164" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B165" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="B166" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="B167" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="B168" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B169" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="B170" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="B171" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="B172" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="B173" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="B174" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="B175" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="B176" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="B177" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="B178" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="B179" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="B180" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="B181">
         <v>330</v>
@@ -3522,7 +3242,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="B182">
         <v>330</v>
@@ -3530,7 +3250,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="B183">
         <v>330</v>
@@ -3538,7 +3258,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="B184">
         <v>330</v>
@@ -3546,103 +3266,103 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="B185" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="B186" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="B187" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="B188" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="B189" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="B190" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="B191" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="B192" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="B193" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="B194" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="B195" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="B196" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="B197">
         <v>32768</v>

</xml_diff>